<commit_message>
Test case for ID #156674345
appetite icon and splash screen validation.
</commit_message>
<xml_diff>
--- a/Appetite - Test Cases - Sprint 7.xlsx
+++ b/Appetite - Test Cases - Sprint 7.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="821"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="821"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint-5" sheetId="122" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>TC1</t>
   </si>
@@ -152,53 +152,25 @@
     <t>TC7</t>
   </si>
   <si>
-    <t>Style/Theme: Check if new theme was applied</t>
+    <t>Animation: Splash screen</t>
   </si>
   <si>
-    <t>Style/Theme: Check if main image appears in the selected restaurant header</t>
+    <t>Icon: check if icon is displayed</t>
   </si>
   <si>
-    <t>Style/Theme: Check if the main image disappear when the header is scrolled up</t>
+    <t>Check if appetite icon appears in the device's screen</t>
   </si>
   <si>
-    <t>Style/Theme: Check search feature in the list</t>
+    <t>Appetite icon (a fork with a small tomato in a red background) appears in the device's screen.</t>
   </si>
   <si>
-    <t>04/10/2018</t>
+    <t>04/17/2018</t>
   </si>
   <si>
-    <t>Style/Theme: Check clear search in the list</t>
+    <t>Push the appetite icon</t>
   </si>
   <si>
-    <t>1. Select one restaurant from the list
-2. Scroll up the image on the header</t>
-  </si>
-  <si>
-    <t>Open the application</t>
-  </si>
-  <si>
-    <t>Now the header background is red</t>
-  </si>
-  <si>
-    <t>The restaurant (if applicable) will be filtered in the list as the user types the name</t>
-  </si>
-  <si>
-    <t>The list of restaurant will show the list of restaurants without any filter.</t>
-  </si>
-  <si>
-    <t>On the restaurant list, click on the magnifier and type the name of the restaurant</t>
-  </si>
-  <si>
-    <t>On the restaurant list, click on the magnifier, type the name and then, delete the field</t>
-  </si>
-  <si>
-    <t>The main image will appear as header background</t>
-  </si>
-  <si>
-    <t>Select one restaurant from the list</t>
-  </si>
-  <si>
-    <t>The header will replace the background image with a red background color</t>
+    <t>Splash screen shows appetite's logo raising from the bottom.</t>
   </si>
 </sst>
 </file>
@@ -880,15 +852,24 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -921,15 +902,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3537,8 +3509,8 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3559,24 +3531,24 @@
       <c r="A2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>25</v>
@@ -3588,9 +3560,9 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
@@ -3604,20 +3576,20 @@
         <v>19</v>
       </c>
       <c r="D4" s="48">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -3626,60 +3598,60 @@
       <c r="J5" s="41"/>
     </row>
     <row r="6" spans="1:10" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="56" t="s">
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="54" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="31" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="53"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="67"/>
+        <v>34</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="38" t="s">
         <v>30</v>
       </c>
@@ -3691,21 +3663,21 @@
       </c>
       <c r="J8" s="38"/>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="67"/>
+        <v>37</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="38" t="s">
         <v>30</v>
       </c>
@@ -3717,82 +3689,46 @@
       </c>
       <c r="J9" s="38"/>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="38" t="s">
-        <v>24</v>
-      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="38"/>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>24</v>
-      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="38"/>
     </row>
-    <row r="12" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="38" t="s">
-        <v>24</v>
-      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
@@ -3801,9 +3737,9 @@
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
       <c r="G13" s="38"/>
       <c r="H13" s="50"/>
       <c r="I13" s="38"/>
@@ -3815,9 +3751,9 @@
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="67"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
       <c r="G14" s="38"/>
       <c r="H14" s="50"/>
       <c r="I14" s="38"/>
@@ -3825,14 +3761,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:F11"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="H2:J2"/>
@@ -3845,6 +3773,14 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:F7"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D11:F11"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3956,7 +3892,7 @@
       </c>
       <c r="D8" s="35">
         <f>'Sprint-5'!B3</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="34">
         <f>'Sprint-5'!B4</f>
@@ -3968,7 +3904,7 @@
       </c>
       <c r="G8" s="35">
         <f>'Sprint-5'!D4</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -3988,7 +3924,7 @@
       </c>
       <c r="D10" s="25">
         <f>SUM(D6:D9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" s="25">
         <f>SUM(E6:E9)</f>
@@ -4000,7 +3936,7 @@
       </c>
       <c r="G10" s="26">
         <f>SUM(G6:G9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>